<commit_message>
add black and scholes
</commit_message>
<xml_diff>
--- a/data/market_20240731.xlsx
+++ b/data/market_20240731.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carap\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\tQuant_testQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88172AC0-B27D-4123-9C49-CACB2C5E05CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85DCC3A-1DC2-4021-A16A-2F98C2C597DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19740" windowHeight="20985" xr2:uid="{900E2547-3339-4A67-8F2C-B13B04883E43}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{900E2547-3339-4A67-8F2C-B13B04883E43}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="curves" sheetId="1" r:id="rId1"/>
+    <sheet name="vols" sheetId="2" r:id="rId2"/>
+    <sheet name="spot" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">vols!$A$1:$F$26</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="128">
   <si>
     <t>Dp</t>
   </si>
@@ -400,14 +405,34 @@
   </si>
   <si>
     <t>Os</t>
+  </si>
+  <si>
+    <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>tenor</t>
+  </si>
+  <si>
+    <t>eq</t>
+  </si>
+  <si>
+    <t>strike</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>EUR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -451,13 +476,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -776,13 +805,13 @@
   <dimension ref="A1:J231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B63"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" customWidth="1"/>
     <col min="6" max="6" width="13.140625" style="5" bestFit="1" customWidth="1"/>
@@ -5415,4 +5444,597 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932CC4A9-7DAE-4DBA-B2D5-679B1DC28B32}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D2" s="8">
+        <v>30</v>
+      </c>
+      <c r="E2">
+        <v>0.6</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D3" s="8">
+        <v>60</v>
+      </c>
+      <c r="E3">
+        <v>0.6</v>
+      </c>
+      <c r="F3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D4" s="8">
+        <v>90</v>
+      </c>
+      <c r="E4">
+        <v>0.6</v>
+      </c>
+      <c r="F4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D5" s="8">
+        <v>180</v>
+      </c>
+      <c r="E5">
+        <v>0.6</v>
+      </c>
+      <c r="F5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D6" s="8">
+        <v>360</v>
+      </c>
+      <c r="E6">
+        <v>0.6</v>
+      </c>
+      <c r="F6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D7" s="8">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>0.8</v>
+      </c>
+      <c r="F7">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D8" s="8">
+        <v>60</v>
+      </c>
+      <c r="E8">
+        <v>0.8</v>
+      </c>
+      <c r="F8">
+        <v>0.21000000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D9" s="8">
+        <v>90</v>
+      </c>
+      <c r="E9">
+        <v>0.8</v>
+      </c>
+      <c r="F9">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D10" s="8">
+        <v>180</v>
+      </c>
+      <c r="E10">
+        <v>0.8</v>
+      </c>
+      <c r="F10">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D11" s="8">
+        <v>360</v>
+      </c>
+      <c r="E11">
+        <v>0.8</v>
+      </c>
+      <c r="F11">
+        <v>0.41000000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D12" s="9">
+        <v>30</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D13" s="8">
+        <v>60</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0.22000000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D14" s="9">
+        <v>90</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D15" s="9">
+        <v>180</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D16" s="9">
+        <v>360</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0.42000000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D17" s="9">
+        <v>30</v>
+      </c>
+      <c r="E17">
+        <v>1.2</v>
+      </c>
+      <c r="F17">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D18" s="8">
+        <v>60</v>
+      </c>
+      <c r="E18">
+        <v>1.2</v>
+      </c>
+      <c r="F18">
+        <v>0.23000000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D19" s="9">
+        <v>90</v>
+      </c>
+      <c r="E19">
+        <v>1.2</v>
+      </c>
+      <c r="F19">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D20" s="9">
+        <v>180</v>
+      </c>
+      <c r="E20">
+        <v>1.2</v>
+      </c>
+      <c r="F20">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D21" s="9">
+        <v>360</v>
+      </c>
+      <c r="E21">
+        <v>1.2</v>
+      </c>
+      <c r="F21">
+        <v>0.43000000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D22" s="9">
+        <v>30</v>
+      </c>
+      <c r="E22">
+        <v>1.4</v>
+      </c>
+      <c r="F22">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D23" s="8">
+        <v>60</v>
+      </c>
+      <c r="E23">
+        <v>1.4</v>
+      </c>
+      <c r="F23">
+        <v>0.24000000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D24" s="9">
+        <v>90</v>
+      </c>
+      <c r="E24">
+        <v>1.4</v>
+      </c>
+      <c r="F24">
+        <v>0.29000000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D25" s="9">
+        <v>180</v>
+      </c>
+      <c r="E25">
+        <v>1.4</v>
+      </c>
+      <c r="F25">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="1">
+        <v>45504</v>
+      </c>
+      <c r="D26" s="9">
+        <v>360</v>
+      </c>
+      <c r="E26">
+        <v>1.4</v>
+      </c>
+      <c r="F26">
+        <v>0.44000000000000006</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC6F3CA-B850-4796-99B5-8F434E69FB01}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="5">
+        <v>127.62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>